<commit_message>
final changes to excel file for sprint one, adding sprint review
</commit_message>
<xml_diff>
--- a/Documentation/Team_M2JC_Report.xlsx
+++ b/Documentation/Team_M2JC_Report.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="6940" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="6940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="163">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -155,15 +155,6 @@
     <t>GitHub Repository:</t>
   </si>
   <si>
-    <t>Bring pizza to our meetings</t>
-  </si>
-  <si>
-    <t>Leaving leftover pizza on the counter</t>
-  </si>
-  <si>
-    <t>Bring silverware for everyone</t>
-  </si>
-  <si>
     <t>Marriage should not occur during marriage to another spouse</t>
   </si>
   <si>
@@ -536,16 +527,28 @@
     <t>Yet to Start</t>
   </si>
   <si>
-    <t>continious integration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Anyone of us can update the burndown chart, whenever they commit changes, and update the actual time spent coding the userstories.                                          2. More decsiplin will be enforced, so each member finish, and integrate it by Sat, so if any issue occure, it allows us time to fix it.                                                                3. As the project grows bigger, and gets more complex, the team members were confused about the structure of the project, but after the sprint review, we decided to adopt encapsulation,because it will make the project more orgnized,less effort and help in future development. Files will be orgnized as unittest.py, userstories.py, and gedcomefile.py which includes the basis for the gedcom file. </t>
-  </si>
-  <si>
     <t>not integrating your code</t>
   </si>
   <si>
     <t>not writing comments</t>
+  </si>
+  <si>
+    <t>Update Excel file once done with coding with the new values</t>
+  </si>
+  <si>
+    <t>continious integration : one intergation review to be done every Saturday during the group meeting</t>
+  </si>
+  <si>
+    <t>Frequently talking to the partners and one weekly meeting (every Saturday) to check hoe everything is going.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cheking on how everyone is doing with their user story and helping each other </t>
+  </si>
+  <si>
+    <t>unstructured code: we're working on making a better structure to the code (introducing encansulation)</t>
+  </si>
+  <si>
+    <t>maintaining better documentation and minutes during our meetings</t>
   </si>
 </sst>
 </file>
@@ -740,7 +743,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -806,9 +809,6 @@
     <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -818,10 +818,16 @@
     <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="65">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1978,7 +1984,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -2011,70 +2017,70 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="B3" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="B3" s="24" t="s">
-        <v>141</v>
-      </c>
       <c r="C3" s="24" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" s="23" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" s="23" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" s="23" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D6" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="E6" s="24" t="s">
         <v>152</v>
-      </c>
-      <c r="E6" s="24" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -2134,37 +2140,37 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>0</v>
@@ -2187,7 +2193,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B15" s="7">
         <v>41065</v>
@@ -2203,7 +2209,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B16" s="7">
         <v>41078</v>
@@ -2228,7 +2234,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B17" s="7">
         <v>41092</v>
@@ -2253,7 +2259,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="4" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B18" s="7">
         <v>41106</v>
@@ -2278,7 +2284,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B19" s="7">
         <v>41120</v>
@@ -2313,69 +2319,69 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+    <sheetView zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" style="38"/>
-    <col min="2" max="2" width="16.6640625" style="39" customWidth="1"/>
-    <col min="3" max="3" width="12.5" style="39" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" style="39" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" style="39" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="40" customWidth="1"/>
-    <col min="7" max="16384" width="11.1640625" style="39"/>
+    <col min="1" max="1" width="11.1640625" style="37"/>
+    <col min="2" max="2" width="16.6640625" style="38" customWidth="1"/>
+    <col min="3" max="3" width="12.5" style="38" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" style="38" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" style="38" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="39" customWidth="1"/>
+    <col min="7" max="16384" width="11.1640625" style="38"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="36" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="35" t="s">
+    <row r="1" spans="1:6" s="35" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="36" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A2" s="38">
+      <c r="A2" s="37">
         <v>41535</v>
       </c>
-      <c r="B2" s="39">
+      <c r="B2" s="38">
         <v>36</v>
       </c>
-      <c r="D2" s="39">
+      <c r="D2" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A3" s="38">
+      <c r="A3" s="37">
         <v>41549</v>
       </c>
-      <c r="B3" s="39">
+      <c r="B3" s="38">
         <v>30</v>
       </c>
-      <c r="C3" s="39">
+      <c r="C3" s="38">
         <v>8</v>
       </c>
-      <c r="D3" s="39">
+      <c r="D3" s="38">
         <v>134</v>
       </c>
-      <c r="E3" s="42">
+      <c r="E3" s="40">
         <v>850</v>
       </c>
-      <c r="F3" s="40">
+      <c r="F3" s="39">
         <f>(D3-D2)/E3*60</f>
         <v>9.4588235294117649</v>
       </c>
@@ -2390,10 +2396,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2440,13 +2446,13 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>25</v>
@@ -2469,27 +2475,27 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="13" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="34">
+      <c r="E3" s="33">
         <v>75</v>
       </c>
-      <c r="F3" s="34">
+      <c r="F3" s="33">
         <v>60</v>
       </c>
       <c r="G3" s="13">
         <v>20</v>
       </c>
-      <c r="H3" s="34">
+      <c r="H3" s="33">
         <v>30</v>
       </c>
       <c r="I3" s="16">
@@ -2498,27 +2504,27 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="13" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="34">
+      <c r="E4" s="33">
         <v>75</v>
       </c>
-      <c r="F4" s="34">
+      <c r="F4" s="33">
         <v>60</v>
       </c>
       <c r="G4" s="13">
         <v>21</v>
       </c>
-      <c r="H4" s="34">
+      <c r="H4" s="33">
         <v>500</v>
       </c>
       <c r="I4" s="16">
@@ -2527,13 +2533,13 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>25</v>
@@ -2556,13 +2562,13 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="13" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>25</v>
@@ -2585,13 +2591,13 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="13" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>25</v>
@@ -2614,13 +2620,13 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="13" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D8" s="13" t="s">
         <v>25</v>
@@ -2643,13 +2649,13 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="13" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D9" s="13" t="s">
         <v>25</v>
@@ -2693,50 +2699,55 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="273" x14ac:dyDescent="0.15">
-      <c r="B15" s="33" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B15" s="17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B16" s="41" t="s">
+        <v>160</v>
+      </c>
+      <c r="I16" s="4"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B17" s="41" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B18" s="42" t="s">
         <v>159</v>
       </c>
-      <c r="I15" s="4"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B16" s="17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B17" s="33" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B18" s="18" t="s">
-        <v>33</v>
-      </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B19" s="33" t="s">
+      <c r="B19" s="41" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="43" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B21" s="33" t="s">
-        <v>32</v>
+      <c r="B21" s="41" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B22" s="41" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B23" s="18" t="s">
-        <v>161</v>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" ht="26" x14ac:dyDescent="0.15">
+      <c r="B24" s="18" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -2790,16 +2801,16 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="13" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="C2" s="34" t="s">
-        <v>140</v>
+        <v>55</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>137</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E2" s="13">
         <v>60</v>
@@ -2813,16 +2824,16 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="13" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E3" s="13">
         <v>50</v>
@@ -2836,16 +2847,16 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="13" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="C4" s="34" t="s">
-        <v>137</v>
+        <v>58</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>134</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E4" s="13">
         <v>90</v>
@@ -2859,16 +2870,16 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="13" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" s="34" t="s">
-        <v>140</v>
+        <v>59</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>137</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E5" s="13">
         <v>88</v>
@@ -2882,16 +2893,16 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="13" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E6" s="13">
         <v>50</v>
@@ -2905,16 +2916,16 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="13" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" s="34" t="s">
-        <v>139</v>
+        <v>62</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>136</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E7" s="13">
         <v>50</v>
@@ -2928,16 +2939,16 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="13" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8" s="34" t="s">
-        <v>138</v>
+        <v>63</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>135</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E8" s="13">
         <v>50</v>
@@ -2950,17 +2961,17 @@
       <c r="I8" s="13"/>
     </row>
     <row r="9" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="34" t="s">
-        <v>107</v>
+      <c r="A9" s="33" t="s">
+        <v>104</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E9" s="13">
         <v>50</v>
@@ -3022,86 +3033,86 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="13" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="13" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="13" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="13" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="13" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:9" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A7" s="13" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
@@ -3111,30 +3122,30 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="13" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="13" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.15">
@@ -3207,114 +3218,114 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="13" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="13" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="13" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="13" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="13" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="13" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="13" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="13" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.15">
@@ -3359,277 +3370,277 @@
   <sheetData>
     <row r="1" spans="1:3" s="28" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="28" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A2" s="30" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A3" s="30" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A4" s="30" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="48" x14ac:dyDescent="0.15">
       <c r="A5" s="30" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="64" x14ac:dyDescent="0.15">
       <c r="A6" s="30" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A7" s="30" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A8" s="30" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C8" s="31" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A9" s="30" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A10" s="30" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B10" s="30" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A11" s="30" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A12" s="30" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B12" s="30" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A13" s="30" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B13" s="30" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A14" s="30" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B14" s="30" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A15" s="30" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B15" s="30" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A16" s="30" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B16" s="30" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="48" x14ac:dyDescent="0.15">
       <c r="A17" s="30" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B17" s="30" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A18" s="30" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B18" s="30" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="128" x14ac:dyDescent="0.15">
       <c r="A19" s="30" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B19" s="30" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A20" s="30" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B20" s="30" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A21" s="30" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B21" s="30" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A22" s="30" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B22" s="30" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A23" s="30" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B23" s="30" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A24" s="30" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B24" s="30" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A25" s="30" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B25" s="30" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="16" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Updated XL with user story 11
</commit_message>
<xml_diff>
--- a/Documentation/Team_M2JC_Report.xlsx
+++ b/Documentation/Team_M2JC_Report.xlsx
@@ -743,7 +743,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -829,6 +829,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1000,11 +1003,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="407744360"/>
-        <c:axId val="407741616"/>
+        <c:axId val="430483256"/>
+        <c:axId val="430483648"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="407744360"/>
+        <c:axId val="430483256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1014,14 +1017,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="407741616"/>
+        <c:crossAx val="430483648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="407741616"/>
+        <c:axId val="430483648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1032,7 +1035,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="407744360"/>
+        <c:crossAx val="430483256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1119,11 +1122,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="407744752"/>
-        <c:axId val="407746320"/>
+        <c:axId val="430477376"/>
+        <c:axId val="430476592"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="407744752"/>
+        <c:axId val="430477376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1133,14 +1136,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="407746320"/>
+        <c:crossAx val="430476592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="407746320"/>
+        <c:axId val="430476592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1151,7 +1154,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="407744752"/>
+        <c:crossAx val="430477376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1188,7 +1191,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1226,7 +1229,7 @@
         <xdr:cNvPr id="3" name="Rectangular Callout 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1301,7 +1304,7 @@
         <xdr:cNvPr id="4" name="Rectangular Callout 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1366,7 +1369,7 @@
         <xdr:cNvPr id="5" name="Rectangular Callout 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1435,7 +1438,7 @@
         <xdr:cNvPr id="6" name="Rectangular Callout 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1505,7 +1508,7 @@
         <xdr:cNvPr id="7" name="Rectangular Callout 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1574,7 +1577,7 @@
         <xdr:cNvPr id="8" name="Rectangular Callout 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1644,7 +1647,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2865,7 +2868,7 @@
         <v>134</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="E4" s="13">
         <v>90</v>
@@ -2873,9 +2876,15 @@
       <c r="F4" s="13">
         <v>60</v>
       </c>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
+      <c r="G4" s="13">
+        <v>34</v>
+      </c>
+      <c r="H4" s="13">
+        <v>240</v>
+      </c>
+      <c r="I4" s="45">
+        <v>41563</v>
+      </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="13" t="s">

</xml_diff>

<commit_message>
Update the Sprint2 demonstrating program Update XL
</commit_message>
<xml_diff>
--- a/Documentation/Team_M2JC_Report.xlsx
+++ b/Documentation/Team_M2JC_Report.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julie\Documents\GitHub\555\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\我的文档\OneDrive\课程相关\17Fall\CS 555\Project\555\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="14" documentId="336B58AE5F9C803DDC81F95743D877899484DB8D" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{172FCE81-D2FC-49EF-AB9C-C2FDE7BD8337}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="6940" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="19200" windowHeight="6936" tabRatio="500" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId7"/>
     <sheet name="Project Backlog" sheetId="11" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -554,12 +555,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -652,6 +653,17 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -743,7 +755,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -780,9 +792,6 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -828,79 +837,92 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="65">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="64" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -916,9 +938,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="1"/>
-  <c:lang val="en-US"/>
+  <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -987,7 +1009,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-FC8B-423E-BCE0-97BCA44D3CBF}"/>
             </c:ext>
@@ -1053,9 +1075,9 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="1"/>
-  <c:lang val="en-US"/>
+  <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1106,7 +1128,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-8DC9-401C-B8F7-DDA8A66F6D29}"/>
             </c:ext>
@@ -1191,7 +1213,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1229,7 +1251,7 @@
         <xdr:cNvPr id="3" name="Rectangular Callout 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1304,7 +1326,7 @@
         <xdr:cNvPr id="4" name="Rectangular Callout 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1369,7 +1391,7 @@
         <xdr:cNvPr id="5" name="Rectangular Callout 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1438,7 +1460,7 @@
         <xdr:cNvPr id="6" name="Rectangular Callout 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1508,7 +1530,7 @@
         <xdr:cNvPr id="7" name="Rectangular Callout 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1577,7 +1599,7 @@
         <xdr:cNvPr id="8" name="Rectangular Callout 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1647,7 +1669,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1987,128 +2009,128 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.15234375" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="11.1796875" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.84375" style="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.84375" style="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.4609375" style="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32" style="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.4609375" style="24" customWidth="1"/>
-    <col min="6" max="16384" width="11.15234375" style="24"/>
+    <col min="1" max="1" width="7.81640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.81640625" style="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" style="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32" style="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.453125" style="23" customWidth="1"/>
+    <col min="6" max="16384" width="11.1796875" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="22" customFormat="1">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="20" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="23" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="22" t="s">
         <v>135</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="23" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="23" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="23" t="s">
         <v>143</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="23" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="23" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="23" t="s">
         <v>144</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="23" t="s">
         <v>145</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="23" t="s">
         <v>146</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="23" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="23" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="22" t="s">
         <v>137</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="23" t="s">
         <v>147</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="23" t="s">
         <v>149</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="23" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="16.5">
-      <c r="D9" s="22" t="s">
+    <row r="9" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="D9" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="24">
+      <c r="E9" s="23">
         <v>555</v>
       </c>
-      <c r="G9" s="25"/>
-    </row>
-    <row r="10" spans="1:8" ht="16.5">
-      <c r="G10" s="26"/>
-      <c r="H10" s="27"/>
-    </row>
-    <row r="11" spans="1:8" ht="16.5">
-      <c r="G11" s="26"/>
-      <c r="H11" s="27"/>
-    </row>
-    <row r="12" spans="1:8" ht="16.5">
-      <c r="G12" s="26"/>
-      <c r="H12" s="27"/>
+      <c r="G9" s="24"/>
+    </row>
+    <row r="10" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="G10" s="25"/>
+      <c r="H10" s="26"/>
+    </row>
+    <row r="11" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="G11" s="25"/>
+      <c r="H11" s="26"/>
+    </row>
+    <row r="12" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="G12" s="25"/>
+      <c r="H12" s="26"/>
     </row>
   </sheetData>
   <sortState ref="A3:D5">
@@ -2116,10 +2138,10 @@
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E4" r:id="rId1"/>
-    <hyperlink ref="E5" r:id="rId2"/>
-    <hyperlink ref="E6" r:id="rId3"/>
-    <hyperlink ref="E3" r:id="rId4"/>
+    <hyperlink ref="E4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E3" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2127,54 +2149,54 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.15234375" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="11.1796875" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.15234375" style="4"/>
-    <col min="2" max="2" width="9.4609375" customWidth="1"/>
-    <col min="3" max="3" width="15.84375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.3046875" customWidth="1"/>
-    <col min="5" max="5" width="6.84375" customWidth="1"/>
-    <col min="6" max="6" width="12.4609375" style="6" customWidth="1"/>
+    <col min="1" max="1" width="11.1796875" style="4"/>
+    <col min="2" max="2" width="9.453125" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.26953125" customWidth="1"/>
+    <col min="5" max="5" width="6.81640625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="2" customFormat="1">
+    <row r="14" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>120</v>
       </c>
@@ -2197,7 +2219,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>121</v>
       </c>
@@ -2213,7 +2235,7 @@
       <c r="F15" s="8"/>
       <c r="G15" s="6"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>122</v>
       </c>
@@ -2238,7 +2260,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>123</v>
       </c>
@@ -2263,7 +2285,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>124</v>
       </c>
@@ -2288,7 +2310,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>125</v>
       </c>
@@ -2322,72 +2344,72 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.15234375" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="11.1796875" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.15234375" style="37"/>
-    <col min="2" max="2" width="16.69140625" style="38" customWidth="1"/>
-    <col min="3" max="3" width="12.4609375" style="38" customWidth="1"/>
-    <col min="4" max="4" width="7.15234375" style="38" customWidth="1"/>
-    <col min="5" max="5" width="6.84375" style="38" customWidth="1"/>
-    <col min="6" max="6" width="12.4609375" style="39" customWidth="1"/>
-    <col min="7" max="16384" width="11.15234375" style="38"/>
+    <col min="1" max="1" width="11.1796875" style="36"/>
+    <col min="2" max="2" width="16.7265625" style="37" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" style="37" customWidth="1"/>
+    <col min="4" max="4" width="7.1796875" style="37" customWidth="1"/>
+    <col min="5" max="5" width="6.81640625" style="37" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="38" customWidth="1"/>
+    <col min="7" max="16384" width="11.1796875" style="37"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="35" customFormat="1">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:6" s="34" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="35" t="s">
+      <c r="E1" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="35" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="37">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="36">
         <v>41535</v>
       </c>
-      <c r="B2" s="38">
+      <c r="B2" s="37">
         <v>36</v>
       </c>
-      <c r="D2" s="38">
+      <c r="D2" s="37">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="37">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="36">
         <v>41549</v>
       </c>
-      <c r="B3" s="38">
+      <c r="B3" s="37">
         <v>30</v>
       </c>
-      <c r="C3" s="38">
+      <c r="C3" s="37">
         <v>8</v>
       </c>
-      <c r="D3" s="38">
+      <c r="D3" s="37">
         <v>134</v>
       </c>
-      <c r="E3" s="40">
+      <c r="E3" s="39">
         <v>850</v>
       </c>
-      <c r="F3" s="39">
+      <c r="F3" s="38">
         <f>(D3-D2)/E3*60</f>
         <v>9.4588235294117649</v>
       </c>
@@ -2401,27 +2423,27 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.15234375" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="11.1796875" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.15234375" style="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.69140625" customWidth="1"/>
+    <col min="2" max="2" width="32.1796875" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7265625" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.3046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.15234375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.4609375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.3046875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.15234375" style="3"/>
+    <col min="5" max="5" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.1796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>9</v>
       </c>
@@ -2450,7 +2472,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>83</v>
       </c>
@@ -2479,7 +2501,7 @@
         <v>41542</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>84</v>
       </c>
@@ -2492,23 +2514,23 @@
       <c r="D3" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="33">
+      <c r="E3" s="32">
         <v>75</v>
       </c>
-      <c r="F3" s="33">
+      <c r="F3" s="32">
         <v>60</v>
       </c>
       <c r="G3" s="13">
         <v>20</v>
       </c>
-      <c r="H3" s="33">
+      <c r="H3" s="32">
         <v>30</v>
       </c>
       <c r="I3" s="16">
         <v>41549</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>85</v>
       </c>
@@ -2521,23 +2543,23 @@
       <c r="D4" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="33">
+      <c r="E4" s="32">
         <v>75</v>
       </c>
-      <c r="F4" s="33">
+      <c r="F4" s="32">
         <v>60</v>
       </c>
       <c r="G4" s="13">
         <v>21</v>
       </c>
-      <c r="H4" s="33">
+      <c r="H4" s="32">
         <v>500</v>
       </c>
       <c r="I4" s="16">
         <v>41549</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>86</v>
       </c>
@@ -2566,7 +2588,7 @@
         <v>41541</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>87</v>
       </c>
@@ -2595,7 +2617,7 @@
         <v>41541</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
         <v>88</v>
       </c>
@@ -2624,7 +2646,7 @@
         <v>41547</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
         <v>89</v>
       </c>
@@ -2653,7 +2675,7 @@
         <v>41541</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
         <v>90</v>
       </c>
@@ -2682,76 +2704,76 @@
         <v>41542</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
-      <c r="E10" s="20">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E10" s="19">
         <f>SUM(E2:E9)</f>
         <v>600</v>
       </c>
-      <c r="F10" s="20">
+      <c r="F10" s="19">
         <f>SUM(F2:F9)</f>
         <v>480</v>
       </c>
-      <c r="G10" s="20">
+      <c r="G10" s="19">
         <f>SUM(G2:G9)</f>
         <v>134</v>
       </c>
-      <c r="H10" s="20">
+      <c r="H10" s="19">
         <f>SUM(H2:H9)</f>
         <v>850</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B14" s="17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15" s="17" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
-      <c r="B16" s="41" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B16" s="40" t="s">
         <v>160</v>
       </c>
       <c r="I16" s="4"/>
     </row>
-    <row r="17" spans="2:2">
-      <c r="B17" s="41" t="s">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="40" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="18" spans="2:2">
-      <c r="B18" s="42" t="s">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="41" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="19" spans="2:2">
-      <c r="B19" s="41" t="s">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="40" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="20" spans="2:2">
-      <c r="B20" s="43" t="s">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B20" s="42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="2:2">
-      <c r="B21" s="41" t="s">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B21" s="40" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="22" spans="2:2">
-      <c r="B22" s="41" t="s">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B22" s="40" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="23" spans="2:2">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B23" s="18" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="24" spans="2:2" ht="27">
+    <row r="24" spans="2:2" ht="25.2" x14ac:dyDescent="0.2">
       <c r="B24" s="18" t="s">
         <v>162</v>
       </c>
@@ -2764,238 +2786,261 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.15234375" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="11.1796875" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="25.4609375" style="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1796875" style="45"/>
+    <col min="2" max="2" width="25.453125" style="49" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="11.1796875" style="45"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="43" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="13" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="46" t="s">
         <v>137</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="46" t="s">
         <v>154</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2" s="46">
         <v>60</v>
       </c>
-      <c r="F2" s="13">
+      <c r="F2" s="46">
         <v>60</v>
       </c>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="13" t="s">
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="46" t="s">
         <v>92</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="46" t="s">
         <v>134</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="46" t="s">
         <v>163</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="46">
         <v>50</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="46">
         <v>60</v>
       </c>
-      <c r="G3" s="13">
+      <c r="G3" s="46">
         <v>10</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H3" s="46">
         <v>60</v>
       </c>
-      <c r="I3" s="44">
+      <c r="I3" s="48">
         <v>41563</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="13" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="46" t="s">
         <v>93</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="46" t="s">
         <v>134</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="46" t="s">
         <v>163</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="46">
         <v>90</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="46">
         <v>60</v>
       </c>
-      <c r="G4" s="13">
+      <c r="G4" s="46">
         <v>34</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H4" s="46">
         <v>240</v>
       </c>
-      <c r="I4" s="45">
+      <c r="I4" s="48">
         <v>41563</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="13" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="46" t="s">
         <v>94</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="46" t="s">
         <v>137</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="46" t="s">
         <v>154</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="46">
         <v>88</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="46">
         <v>90</v>
       </c>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="13" t="s">
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="46" t="s">
         <v>96</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="47" t="s">
         <v>129</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="46" t="s">
         <v>136</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="46" t="s">
+        <v>163</v>
+      </c>
+      <c r="E6" s="46">
+        <v>50</v>
+      </c>
+      <c r="F6" s="46">
+        <v>120</v>
+      </c>
+      <c r="G6" s="46">
+        <v>40</v>
+      </c>
+      <c r="H6" s="46">
+        <v>60</v>
+      </c>
+      <c r="I6" s="48">
+        <v>41561</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="46" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" s="47" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="46" t="s">
+        <v>136</v>
+      </c>
+      <c r="D7" s="46" t="s">
+        <v>163</v>
+      </c>
+      <c r="E7" s="46">
+        <v>50</v>
+      </c>
+      <c r="F7" s="46">
+        <v>60</v>
+      </c>
+      <c r="G7" s="46">
+        <v>50</v>
+      </c>
+      <c r="H7" s="46">
+        <v>80</v>
+      </c>
+      <c r="I7" s="48">
+        <v>41561</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="46" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" s="47" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="46" t="s">
+        <v>135</v>
+      </c>
+      <c r="D8" s="46" t="s">
         <v>154</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E8" s="46">
         <v>50</v>
       </c>
-      <c r="F6" s="13">
-        <v>120</v>
-      </c>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="C7" s="33" t="s">
-        <v>136</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="E7" s="13">
+      <c r="F8" s="46">
+        <v>90</v>
+      </c>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
+    </row>
+    <row r="9" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="46" t="s">
+        <v>104</v>
+      </c>
+      <c r="B9" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="46" t="s">
+        <v>135</v>
+      </c>
+      <c r="D9" s="46" t="s">
+        <v>163</v>
+      </c>
+      <c r="E9" s="46">
         <v>50</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F9" s="46">
         <v>60</v>
       </c>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" s="33" t="s">
-        <v>135</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="E8" s="13">
+      <c r="G9" s="46">
+        <v>35</v>
+      </c>
+      <c r="H9" s="46">
         <v>50</v>
       </c>
-      <c r="F8" s="13">
-        <v>90</v>
-      </c>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-    </row>
-    <row r="9" spans="1:9" s="13" customFormat="1">
-      <c r="A9" s="33" t="s">
-        <v>104</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="E9" s="13">
-        <v>50</v>
-      </c>
-      <c r="F9" s="13">
-        <v>60</v>
+      <c r="I9" s="48">
+        <v>41563</v>
       </c>
     </row>
   </sheetData>
@@ -3006,21 +3051,21 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.84375" style="13"/>
-    <col min="2" max="2" width="26.4609375" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.84375" style="13"/>
+    <col min="1" max="1" width="10.81640625" style="13"/>
+    <col min="2" max="2" width="26.453125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.81640625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
@@ -3049,7 +3094,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>99</v>
       </c>
@@ -3063,7 +3108,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>100</v>
       </c>
@@ -3077,7 +3122,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>101</v>
       </c>
@@ -3091,7 +3136,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>102</v>
       </c>
@@ -3105,7 +3150,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>103</v>
       </c>
@@ -3119,7 +3164,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="7" spans="1:9" customFormat="1">
+    <row r="7" spans="1:9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
         <v>95</v>
       </c>
@@ -3138,7 +3183,7 @@
       <c r="H7" s="13"/>
       <c r="I7" s="13"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
         <v>105</v>
       </c>
@@ -3152,7 +3197,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
         <v>106</v>
       </c>
@@ -3166,20 +3211,20 @@
         <v>154</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
-      <c r="E10" s="20">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E10" s="19">
         <f>SUM(E2:E9)</f>
         <v>0</v>
       </c>
-      <c r="F10" s="20">
+      <c r="F10" s="19">
         <f>SUM(F2:F9)</f>
         <v>0</v>
       </c>
-      <c r="G10" s="20">
+      <c r="G10" s="19">
         <f>SUM(G2:G9)</f>
         <v>0</v>
       </c>
-      <c r="H10" s="20">
+      <c r="H10" s="19">
         <f>SUM(H2:H9)</f>
         <v>0</v>
       </c>
@@ -3191,21 +3236,21 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="E10" sqref="E10:H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.84375" style="13"/>
+    <col min="1" max="1" width="10.81640625" style="13"/>
     <col min="2" max="2" width="26" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.84375" style="13"/>
+    <col min="3" max="16384" width="10.81640625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
@@ -3234,7 +3279,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>107</v>
       </c>
@@ -3248,7 +3293,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>108</v>
       </c>
@@ -3262,7 +3307,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>109</v>
       </c>
@@ -3276,7 +3321,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>110</v>
       </c>
@@ -3290,7 +3335,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>111</v>
       </c>
@@ -3304,7 +3349,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
         <v>112</v>
       </c>
@@ -3318,7 +3363,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
         <v>113</v>
       </c>
@@ -3332,7 +3377,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
         <v>114</v>
       </c>
@@ -3346,20 +3391,20 @@
         <v>154</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
-      <c r="E10" s="20">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E10" s="19">
         <f>SUM(E2:E9)</f>
         <v>0</v>
       </c>
-      <c r="F10" s="20">
+      <c r="F10" s="19">
         <f>SUM(F2:F9)</f>
         <v>0</v>
       </c>
-      <c r="G10" s="20">
+      <c r="G10" s="19">
         <f>SUM(G2:G9)</f>
         <v>0</v>
       </c>
-      <c r="H10" s="20">
+      <c r="H10" s="19">
         <f>SUM(H2:H9)</f>
         <v>0</v>
       </c>
@@ -3371,325 +3416,325 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.15234375" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="11.1796875" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.15234375" style="30"/>
-    <col min="2" max="2" width="28.15234375" style="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.4609375" style="32" customWidth="1"/>
-    <col min="4" max="16384" width="11.15234375" style="30"/>
+    <col min="1" max="1" width="11.1796875" style="29"/>
+    <col min="2" max="2" width="28.1796875" style="29" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.453125" style="31" customWidth="1"/>
+    <col min="4" max="16384" width="11.1796875" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="28" customFormat="1">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:3" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="28" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30">
-      <c r="A2" s="30" t="s">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A2" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="30" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="30">
-      <c r="A3" s="30" t="s">
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A3" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="30" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30">
-      <c r="A4" s="30" t="s">
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A4" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="30" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="45">
-      <c r="A5" s="30" t="s">
+    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+      <c r="A5" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="30" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="45">
-      <c r="A6" s="30" t="s">
+    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+      <c r="A6" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="30" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15">
-      <c r="A7" s="30" t="s">
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A7" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="29" t="s">
         <v>129</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="30" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15">
-      <c r="A8" s="30" t="s">
+    <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A8" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="C8" s="30" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30">
-      <c r="A9" s="30" t="s">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A9" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="30" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15">
-      <c r="A10" s="30" t="s">
+    <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A10" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="C10" s="31" t="s">
+      <c r="C10" s="30" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15">
-      <c r="A11" s="30" t="s">
+    <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A11" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="30" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15">
-      <c r="A12" s="30" t="s">
+    <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A12" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="C12" s="31" t="s">
+      <c r="C12" s="30" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="30">
-      <c r="A13" s="30" t="s">
+    <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A13" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="31" t="s">
+      <c r="C13" s="30" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="30">
-      <c r="A14" s="30" t="s">
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A14" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="30" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="30">
-      <c r="A15" s="30" t="s">
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A15" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="B15" s="30" t="s">
+      <c r="B15" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="C15" s="31" t="s">
+      <c r="C15" s="30" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="30">
-      <c r="A16" s="30" t="s">
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A16" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="C16" s="31" t="s">
+      <c r="C16" s="30" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="45">
-      <c r="A17" s="30" t="s">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A17" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="C17" s="31" t="s">
+      <c r="C17" s="30" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="30">
-      <c r="A18" s="30" t="s">
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A18" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="B18" s="30" t="s">
+      <c r="B18" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="C18" s="31" t="s">
+      <c r="C18" s="30" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="105">
-      <c r="A19" s="30" t="s">
+    <row r="19" spans="1:3" ht="105" x14ac:dyDescent="0.2">
+      <c r="A19" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="C19" s="31" t="s">
+      <c r="C19" s="30" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15">
-      <c r="A20" s="30" t="s">
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A20" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="B20" s="30" t="s">
+      <c r="B20" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="C20" s="31" t="s">
+      <c r="C20" s="30" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30">
-      <c r="A21" s="30" t="s">
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A21" s="29" t="s">
         <v>110</v>
       </c>
-      <c r="B21" s="30" t="s">
+      <c r="B21" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="C21" s="31" t="s">
+      <c r="C21" s="30" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15">
-      <c r="A22" s="30" t="s">
+    <row r="22" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A22" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="C22" s="31" t="s">
+      <c r="C22" s="30" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15">
-      <c r="A23" s="30" t="s">
+    <row r="23" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A23" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="B23" s="30" t="s">
+      <c r="B23" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="C23" s="31" t="s">
+      <c r="C23" s="30" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30">
-      <c r="A24" s="30" t="s">
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A24" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="B24" s="30" t="s">
+      <c r="B24" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="C24" s="31" t="s">
+      <c r="C24" s="30" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15">
-      <c r="A25" s="30" t="s">
+    <row r="25" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A25" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="B25" s="30" t="s">
+      <c r="B25" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="C25" s="31" t="s">
+      <c r="C25" s="30" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15">
-      <c r="C26" s="31"/>
-    </row>
-    <row r="27" spans="1:3" ht="15">
-      <c r="C27" s="31"/>
-    </row>
-    <row r="28" spans="1:3" ht="15">
-      <c r="C28" s="31"/>
-    </row>
-    <row r="29" spans="1:3" ht="15">
-      <c r="C29" s="31"/>
-    </row>
-    <row r="30" spans="1:3" ht="15">
-      <c r="C30" s="31"/>
-    </row>
-    <row r="31" spans="1:3" ht="15">
-      <c r="C31" s="31"/>
-    </row>
-    <row r="32" spans="1:3" ht="15">
-      <c r="C32" s="31"/>
-    </row>
-    <row r="33" spans="3:3" ht="15">
-      <c r="C33" s="31"/>
-    </row>
-    <row r="34" spans="3:3" ht="15">
-      <c r="C34" s="31"/>
-    </row>
-    <row r="35" spans="3:3" ht="15">
-      <c r="C35" s="31"/>
+    <row r="26" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="C26" s="30"/>
+    </row>
+    <row r="27" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="C27" s="30"/>
+    </row>
+    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="C28" s="30"/>
+    </row>
+    <row r="29" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="C29" s="30"/>
+    </row>
+    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="C30" s="30"/>
+    </row>
+    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="C31" s="30"/>
+    </row>
+    <row r="32" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="C32" s="30"/>
+    </row>
+    <row r="33" spans="3:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="C33" s="30"/>
+    </row>
+    <row r="34" spans="3:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="C34" s="30"/>
+    </row>
+    <row r="35" spans="3:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="C35" s="30"/>
     </row>
   </sheetData>
   <phoneticPr fontId="15" type="noConversion"/>

</xml_diff>

<commit_message>
Updated Sprint 2, and 3
</commit_message>
<xml_diff>
--- a/Documentation/Team_M2JC_Report.xlsx
+++ b/Documentation/Team_M2JC_Report.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18528"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\我的文档\OneDrive\课程相关\17Fall\CS 555\Project\555\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maryam\Documents\GitHub\555\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="336B58AE5F9C803DDC81F95743D877899484DB8D" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{172FCE81-D2FC-49EF-AB9C-C2FDE7BD8337}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="19200" windowHeight="6936" tabRatio="500" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="6940" tabRatio="500" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="165">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -134,10 +133,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Coding</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Review Results</t>
   </si>
   <si>
@@ -153,18 +148,6 @@
     <t>GitHub Repository:</t>
   </si>
   <si>
-    <t>Marriage should not occur during marriage to another spouse</t>
-  </si>
-  <si>
-    <t>No more than five siblings should be born at the same time</t>
-  </si>
-  <si>
-    <t>There should be fewer than 15 siblings in a family</t>
-  </si>
-  <si>
-    <t>All male members of a family should have the same last name</t>
-  </si>
-  <si>
     <t>Parents should not marry any of their descendants</t>
   </si>
   <si>
@@ -228,9 +211,6 @@
     <t>Birth before death of parents</t>
   </si>
   <si>
-    <t>Child should be born before death of mother and before 9 months after death of father</t>
-  </si>
-  <si>
     <t>Marriage after 14</t>
   </si>
   <si>
@@ -240,9 +220,6 @@
     <t>Parents not too old</t>
   </si>
   <si>
-    <t>Mother should be less than 60 years older than her children and father should be less than 80 years older than his children</t>
-  </si>
-  <si>
     <t>Siblings spacing</t>
   </si>
   <si>
@@ -270,9 +247,6 @@
     <t>Husband in family should be male and wife in family should be female</t>
   </si>
   <si>
-    <t>All individual IDs should be unique and all family IDs should be unique</t>
-  </si>
-  <si>
     <t>Unique IDs</t>
   </si>
   <si>
@@ -450,9 +424,6 @@
     <t>Multiple births &lt;= 5</t>
   </si>
   <si>
-    <t>Marriage should be at least 14 years after birth of both spouses (parents must be at least 14 years old)</t>
-  </si>
-  <si>
     <t>Birth dates of siblings should be more than 8 months apart or less than 2 days apart (twins may be born one day apart, e.g. 11:59 PM and 12:02 AM the following calendar day)</t>
   </si>
   <si>
@@ -550,6 +521,36 @@
   </si>
   <si>
     <t>Completed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keep Doing: </t>
+  </si>
+  <si>
+    <t>Updating the Burndown Chart</t>
+  </si>
+  <si>
+    <t>Check on how everyone is doing with their user stories, and offer help if needed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Follow TDD Test before Developing </t>
+  </si>
+  <si>
+    <t>Meet every Saturday for sprint review and sprint planning</t>
+  </si>
+  <si>
+    <t>Not defining default time for submission</t>
+  </si>
+  <si>
+    <t>Start Structuring the coding earlier (Thursday)</t>
+  </si>
+  <si>
+    <t>Underestimating implementation time for new user stories: Dividing big ones to manageable small user stories</t>
+  </si>
+  <si>
+    <t>Continuous Integration at each commit</t>
+  </si>
+  <si>
+    <t>Start implementation early</t>
   </si>
 </sst>
 </file>
@@ -560,7 +561,7 @@
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -755,7 +756,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -856,73 +857,79 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="65">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -940,7 +947,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="1"/>
-  <c:lang val="zh-CN"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1077,7 +1084,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="1"/>
-  <c:lang val="zh-CN"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2016,17 +2023,17 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1796875" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.15234375" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="7.81640625" style="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.81640625" style="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.453125" style="23" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.84375" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.84375" style="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.4609375" style="23" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32" style="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.453125" style="23" customWidth="1"/>
-    <col min="6" max="16384" width="11.1796875" style="23"/>
+    <col min="5" max="5" width="20.4609375" style="23" customWidth="1"/>
+    <col min="6" max="16384" width="11.15234375" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="21" customFormat="1">
       <c r="A1" s="20" t="s">
         <v>18</v>
       </c>
@@ -2040,95 +2047,95 @@
         <v>21</v>
       </c>
       <c r="E1" s="20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="16.5">
+      <c r="D9" s="21" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
-        <v>135</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>138</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>139</v>
-      </c>
-      <c r="D3" s="23" t="s">
-        <v>140</v>
-      </c>
-      <c r="E3" s="23" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="22" t="s">
-        <v>134</v>
-      </c>
-      <c r="B4" s="23" t="s">
-        <v>141</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="D4" s="23" t="s">
-        <v>143</v>
-      </c>
-      <c r="E4" s="23" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="22" t="s">
-        <v>136</v>
-      </c>
-      <c r="B5" s="23" t="s">
-        <v>144</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>145</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>146</v>
-      </c>
-      <c r="E5" s="23" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="22" t="s">
-        <v>137</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>147</v>
-      </c>
-      <c r="C6" s="23" t="s">
-        <v>148</v>
-      </c>
-      <c r="D6" s="23" t="s">
-        <v>149</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="D9" s="21" t="s">
-        <v>30</v>
       </c>
       <c r="E9" s="23">
         <v>555</v>
       </c>
       <c r="G9" s="24"/>
     </row>
-    <row r="10" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="16.5">
       <c r="G10" s="25"/>
       <c r="H10" s="26"/>
     </row>
-    <row r="11" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="16.5">
       <c r="G11" s="25"/>
       <c r="H11" s="26"/>
     </row>
-    <row r="12" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="16.5">
       <c r="G12" s="25"/>
       <c r="H12" s="26"/>
     </row>
@@ -2152,53 +2159,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView topLeftCell="A10" zoomScale="150" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1796875" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.15234375" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="11.1796875" style="4"/>
-    <col min="2" max="2" width="9.453125" customWidth="1"/>
-    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.26953125" customWidth="1"/>
-    <col min="5" max="5" width="6.81640625" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="11.15234375" style="4"/>
+    <col min="2" max="2" width="9.4609375" customWidth="1"/>
+    <col min="3" max="3" width="15.84375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.23046875" customWidth="1"/>
+    <col min="5" max="5" width="6.84375" customWidth="1"/>
+    <col min="6" max="6" width="12.4609375" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="4" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+    <row r="6" spans="1:7">
+      <c r="A6" s="4" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="A8" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="2" customFormat="1">
       <c r="A14" s="2" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>0</v>
@@ -2219,9 +2226,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B15" s="7">
         <v>41065</v>
@@ -2235,9 +2242,9 @@
       <c r="F15" s="8"/>
       <c r="G15" s="6"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B16" s="7">
         <v>41078</v>
@@ -2260,9 +2267,9 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7">
       <c r="A17" s="4" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B17" s="7">
         <v>41092</v>
@@ -2285,9 +2292,9 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7">
       <c r="A18" s="4" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="B18" s="7">
         <v>41106</v>
@@ -2310,9 +2317,9 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7">
       <c r="A19" s="4" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B19" s="7">
         <v>41120</v>
@@ -2347,22 +2354,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1796875" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.15234375" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="11.1796875" style="36"/>
-    <col min="2" max="2" width="16.7265625" style="37" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" style="37" customWidth="1"/>
-    <col min="4" max="4" width="7.1796875" style="37" customWidth="1"/>
-    <col min="5" max="5" width="6.81640625" style="37" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="38" customWidth="1"/>
-    <col min="7" max="16384" width="11.1796875" style="37"/>
+    <col min="1" max="1" width="11.15234375" style="36"/>
+    <col min="2" max="2" width="16.69140625" style="37" customWidth="1"/>
+    <col min="3" max="3" width="12.4609375" style="37" customWidth="1"/>
+    <col min="4" max="4" width="7.15234375" style="37" customWidth="1"/>
+    <col min="5" max="5" width="6.84375" style="37" customWidth="1"/>
+    <col min="6" max="6" width="12.4609375" style="38" customWidth="1"/>
+    <col min="7" max="16384" width="11.15234375" style="37"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="34" customFormat="1">
       <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
@@ -2382,7 +2389,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" s="36">
         <v>41535</v>
       </c>
@@ -2393,7 +2400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" s="36">
         <v>41549</v>
       </c>
@@ -2427,23 +2434,23 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1796875" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.15234375" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.1796875" style="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.7265625" customWidth="1"/>
-    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.1796875" style="3"/>
+    <col min="2" max="2" width="32.15234375" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.69140625" customWidth="1"/>
+    <col min="4" max="4" width="8.69140625" customWidth="1"/>
+    <col min="5" max="5" width="8.23046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.15234375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.4609375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.23046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.15234375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" s="12" t="s">
         <v>9</v>
       </c>
@@ -2472,18 +2479,18 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9">
       <c r="A2" s="13" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>25</v>
+        <v>125</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>154</v>
       </c>
       <c r="E2" s="13">
         <v>75</v>
@@ -2501,18 +2508,18 @@
         <v>41542</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3" s="13" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>25</v>
+        <v>126</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>154</v>
       </c>
       <c r="E3" s="32">
         <v>75</v>
@@ -2530,18 +2537,18 @@
         <v>41549</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4" s="13" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>25</v>
+        <v>126</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>154</v>
       </c>
       <c r="E4" s="32">
         <v>75</v>
@@ -2559,18 +2566,18 @@
         <v>41549</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" s="13" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>25</v>
+        <v>127</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>154</v>
       </c>
       <c r="E5" s="13">
         <v>75</v>
@@ -2588,18 +2595,18 @@
         <v>41541</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="A6" s="13" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>25</v>
+        <v>127</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>154</v>
       </c>
       <c r="E6" s="13">
         <v>75</v>
@@ -2617,18 +2624,18 @@
         <v>41541</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9">
       <c r="A7" s="13" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>25</v>
+        <v>125</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>154</v>
       </c>
       <c r="E7" s="13">
         <v>75</v>
@@ -2646,18 +2653,18 @@
         <v>41547</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9">
       <c r="A8" s="13" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>25</v>
+        <v>128</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>154</v>
       </c>
       <c r="E8" s="13">
         <v>75</v>
@@ -2675,18 +2682,18 @@
         <v>41541</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9">
       <c r="A9" s="13" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>25</v>
+        <v>128</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>154</v>
       </c>
       <c r="E9" s="13">
         <v>75</v>
@@ -2704,7 +2711,7 @@
         <v>41542</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9">
       <c r="E10" s="19">
         <f>SUM(E2:E9)</f>
         <v>600</v>
@@ -2722,60 +2729,60 @@
         <v>850</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9">
       <c r="B14" s="17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="B15" s="17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B15" s="17" t="s">
+    <row r="16" spans="1:9">
+      <c r="B16" s="40" t="s">
+        <v>151</v>
+      </c>
+      <c r="I16" s="4"/>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" s="40" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" s="41" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" s="40" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" s="42" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B16" s="40" t="s">
-        <v>160</v>
-      </c>
-      <c r="I16" s="4"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17" s="40" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B18" s="41" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B19" s="40" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B20" s="42" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:2">
       <c r="B21" s="40" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2">
       <c r="B22" s="40" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2">
       <c r="B23" s="18" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2" ht="25.2" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" ht="27">
       <c r="B24" s="18" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -2787,20 +2794,20 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1796875" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.15234375" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="11.1796875" style="45"/>
-    <col min="2" max="2" width="25.453125" style="49" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="11.1796875" style="45"/>
+    <col min="1" max="1" width="11.15234375" style="45"/>
+    <col min="2" max="2" width="25.4609375" style="49" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="11.15234375" style="45"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" s="43" t="s">
         <v>9</v>
       </c>
@@ -2829,18 +2836,18 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9">
       <c r="A2" s="46" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C2" s="46" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="D2" s="46" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="E2" s="46">
         <v>60</v>
@@ -2849,21 +2856,25 @@
         <v>60</v>
       </c>
       <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H2" s="46">
+        <v>60</v>
+      </c>
+      <c r="I2" s="48">
+        <v>41563</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="46" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C3" s="46" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="D3" s="46" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="E3" s="46">
         <v>50</v>
@@ -2881,18 +2892,18 @@
         <v>41563</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4" s="46" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="B4" s="47" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C4" s="46" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="D4" s="46" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="E4" s="46">
         <v>90</v>
@@ -2910,18 +2921,18 @@
         <v>41563</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" s="46" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B5" s="47" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C5" s="46" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="D5" s="46" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="E5" s="46">
         <v>88</v>
@@ -2930,21 +2941,25 @@
         <v>90</v>
       </c>
       <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H5" s="46">
+        <v>60</v>
+      </c>
+      <c r="I5" s="48">
+        <v>41563</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="46" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B6" s="47" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="C6" s="46" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="D6" s="46" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="E6" s="46">
         <v>50</v>
@@ -2959,21 +2974,21 @@
         <v>60</v>
       </c>
       <c r="I6" s="48">
-        <v>41561</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+        <v>41563</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="46" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B7" s="47" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C7" s="46" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="D7" s="46" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="E7" s="46">
         <v>50</v>
@@ -2988,21 +3003,21 @@
         <v>80</v>
       </c>
       <c r="I7" s="48">
-        <v>41561</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+        <v>41563</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="46" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B8" s="47" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C8" s="46" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="D8" s="46" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="E8" s="46">
         <v>50</v>
@@ -3011,21 +3026,25 @@
         <v>90</v>
       </c>
       <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="46"/>
-    </row>
-    <row r="9" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H8" s="46">
+        <v>60</v>
+      </c>
+      <c r="I8" s="48">
+        <v>41563</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="46" customFormat="1">
       <c r="A9" s="46" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B9" s="47" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C9" s="46" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="D9" s="46" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="E9" s="46">
         <v>50</v>
@@ -3041,12 +3060,96 @@
       </c>
       <c r="I9" s="48">
         <v>41563</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="E10" s="45">
+        <f>SUM(E2:E9)</f>
+        <v>488</v>
+      </c>
+      <c r="F10" s="45">
+        <f>SUM(F2:F9)</f>
+        <v>600</v>
+      </c>
+      <c r="G10" s="45">
+        <f>SUM(G1:G9)</f>
+        <v>169</v>
+      </c>
+      <c r="H10" s="45">
+        <f>SUM(H2:H9)</f>
+        <v>670</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="B13" s="50" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="B14" s="50" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="B15" s="49" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="B16" s="49" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" s="49" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" s="49" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" s="49" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" s="51" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" s="50" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" s="49" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2">
+      <c r="B23" s="49" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" s="49" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="1048576" spans="6:6">
+      <c r="F1048576" s="45">
+        <f>SUM(F2:F1048575)</f>
+        <v>1200</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3055,17 +3158,17 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" style="13"/>
-    <col min="2" max="2" width="26.453125" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.81640625" style="13"/>
+    <col min="1" max="1" width="10.84375" style="13"/>
+    <col min="2" max="2" width="26.4609375" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.84375" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
@@ -3094,131 +3197,177 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9">
       <c r="A2" s="13" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+      <c r="E2" s="13">
+        <v>120</v>
+      </c>
+      <c r="F2" s="13">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="13" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+      <c r="E3" s="13">
+        <v>30</v>
+      </c>
+      <c r="F3" s="13">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="13" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+      <c r="E4" s="13">
+        <v>60</v>
+      </c>
+      <c r="F4" s="13">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="13" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+      <c r="E5" s="13">
+        <v>80</v>
+      </c>
+      <c r="F5" s="13">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="13" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" customFormat="1" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+      <c r="E6" s="13">
+        <v>90</v>
+      </c>
+      <c r="F6" s="13">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" customFormat="1">
       <c r="A7" s="13" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
+        <v>145</v>
+      </c>
+      <c r="E7" s="13">
+        <v>44</v>
+      </c>
+      <c r="F7" s="13">
+        <v>60</v>
+      </c>
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
       <c r="I7" s="13"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9">
       <c r="A8" s="13" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+      <c r="E8" s="13">
+        <v>30</v>
+      </c>
+      <c r="F8" s="13">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="13" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+      <c r="E9" s="13">
+        <v>30</v>
+      </c>
+      <c r="F9" s="13">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="E10" s="19">
         <f>SUM(E2:E9)</f>
-        <v>0</v>
+        <v>484</v>
       </c>
       <c r="F10" s="19">
         <f>SUM(F2:F9)</f>
-        <v>0</v>
+        <v>440</v>
       </c>
       <c r="G10" s="19">
         <f>SUM(G2:G9)</f>
@@ -3243,14 +3392,14 @@
       <selection activeCell="E10" sqref="E10:H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.84375" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" style="13"/>
+    <col min="1" max="1" width="10.84375" style="13"/>
     <col min="2" max="2" width="26" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.81640625" style="13"/>
+    <col min="3" max="16384" width="10.84375" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
@@ -3279,119 +3428,119 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9">
       <c r="A2" s="13" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="13" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="13" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="13" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="13" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="13" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="13" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="13" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="E10" s="19">
         <f>SUM(E2:E9)</f>
         <v>0</v>
@@ -3417,56 +3566,56 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1796875" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.15234375" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="11.1796875" style="29"/>
-    <col min="2" max="2" width="28.1796875" style="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.453125" style="31" customWidth="1"/>
-    <col min="4" max="16384" width="11.1796875" style="29"/>
+    <col min="1" max="1" width="11.15234375" style="29"/>
+    <col min="2" max="2" width="28.15234375" style="29" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.4609375" style="31" customWidth="1"/>
+    <col min="4" max="16384" width="11.15234375" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="27" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="27" customFormat="1">
       <c r="A1" s="27" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B1" s="27" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C1" s="28" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="45">
       <c r="A2" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15">
+      <c r="A3" s="29" t="s">
         <v>91</v>
-      </c>
-      <c r="B2" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" s="30" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A3" s="29" t="s">
-        <v>92</v>
       </c>
       <c r="B3" s="29" t="s">
         <v>57</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15">
       <c r="A4" s="29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B4" s="29" t="s">
         <v>58</v>
@@ -3475,117 +3624,117 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="15">
       <c r="A5" s="29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B5" s="29" t="s">
         <v>59</v>
       </c>
       <c r="C5" s="30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30">
+      <c r="A6" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="29" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.2">
-      <c r="A6" s="29" t="s">
+      <c r="C6" s="30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="30">
+      <c r="A7" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B7" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="30" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="29" t="s">
-        <v>96</v>
-      </c>
-      <c r="B7" s="29" t="s">
-        <v>129</v>
-      </c>
       <c r="C7" s="30" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="30">
       <c r="A8" s="29" t="s">
         <v>97</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="45">
       <c r="A9" s="29" t="s">
         <v>98</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30">
       <c r="A10" s="29" t="s">
         <v>99</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="105">
       <c r="A11" s="29" t="s">
         <v>100</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15">
       <c r="A12" s="29" t="s">
         <v>101</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C12" s="30" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="30">
       <c r="A13" s="29" t="s">
         <v>102</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15">
       <c r="A14" s="29" t="s">
         <v>103</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15">
       <c r="A15" s="29" t="s">
         <v>104</v>
       </c>
@@ -3593,10 +3742,10 @@
         <v>71</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="30">
       <c r="A16" s="29" t="s">
         <v>105</v>
       </c>
@@ -3604,10 +3753,10 @@
         <v>72</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15">
       <c r="A17" s="29" t="s">
         <v>106</v>
       </c>
@@ -3615,126 +3764,38 @@
         <v>73</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A18" s="29" t="s">
-        <v>107</v>
-      </c>
-      <c r="B18" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="C18" s="30" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="105" x14ac:dyDescent="0.2">
-      <c r="A19" s="29" t="s">
-        <v>108</v>
-      </c>
-      <c r="B19" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="C19" s="30" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A20" s="29" t="s">
-        <v>109</v>
-      </c>
-      <c r="B20" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="C20" s="30" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A21" s="29" t="s">
-        <v>110</v>
-      </c>
-      <c r="B21" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="C21" s="30" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A22" s="29" t="s">
-        <v>111</v>
-      </c>
-      <c r="B22" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="C22" s="30" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A23" s="29" t="s">
-        <v>112</v>
-      </c>
-      <c r="B23" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="C23" s="30" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.2">
-      <c r="A24" s="29" t="s">
-        <v>113</v>
-      </c>
-      <c r="B24" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="C24" s="30" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A25" s="29" t="s">
-        <v>114</v>
-      </c>
-      <c r="B25" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="C25" s="30" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="15">
+      <c r="C18" s="30"/>
+    </row>
+    <row r="19" spans="1:3" ht="15">
+      <c r="C19" s="30"/>
+    </row>
+    <row r="20" spans="1:3" ht="15">
+      <c r="C20" s="30"/>
+    </row>
+    <row r="21" spans="1:3" ht="15">
+      <c r="C21" s="30"/>
+    </row>
+    <row r="22" spans="1:3" ht="15">
+      <c r="C22" s="30"/>
+    </row>
+    <row r="23" spans="1:3" ht="15">
+      <c r="C23" s="30"/>
+    </row>
+    <row r="24" spans="1:3" ht="15">
+      <c r="C24" s="30"/>
+    </row>
+    <row r="25" spans="1:3" ht="15">
+      <c r="C25" s="30"/>
+    </row>
+    <row r="26" spans="1:3" ht="15">
       <c r="C26" s="30"/>
     </row>
-    <row r="27" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="15">
       <c r="C27" s="30"/>
-    </row>
-    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="C28" s="30"/>
-    </row>
-    <row r="29" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="C29" s="30"/>
-    </row>
-    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="C30" s="30"/>
-    </row>
-    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="C31" s="30"/>
-    </row>
-    <row r="32" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="C32" s="30"/>
-    </row>
-    <row r="33" spans="3:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="C33" s="30"/>
-    </row>
-    <row r="34" spans="3:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="C34" s="30"/>
-    </row>
-    <row r="35" spans="3:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="C35" s="30"/>
     </row>
   </sheetData>
   <phoneticPr fontId="15" type="noConversion"/>

</xml_diff>

<commit_message>
ADDING SPRINT 4 file
</commit_message>
<xml_diff>
--- a/Documentation/Team_M2JC_Report.xlsx
+++ b/Documentation/Team_M2JC_Report.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="12500" tabRatio="500" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="12500" tabRatio="500" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -2558,7 +2558,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E2" sqref="E2:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3287,7 +3287,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
@@ -3649,8 +3649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3702,6 +3702,12 @@
       <c r="D2" s="23" t="s">
         <v>156</v>
       </c>
+      <c r="E2" s="13">
+        <v>75</v>
+      </c>
+      <c r="F2" s="13">
+        <v>60</v>
+      </c>
     </row>
     <row r="3" spans="1:9" s="29" customFormat="1" ht="16" x14ac:dyDescent="0.15">
       <c r="A3" s="29" t="s">
@@ -3716,6 +3722,12 @@
       <c r="D3" s="23" t="s">
         <v>156</v>
       </c>
+      <c r="E3" s="32">
+        <v>75</v>
+      </c>
+      <c r="F3" s="32">
+        <v>60</v>
+      </c>
     </row>
     <row r="4" spans="1:9" s="29" customFormat="1" ht="16" x14ac:dyDescent="0.15">
       <c r="A4" s="29" t="s">
@@ -3730,6 +3742,12 @@
       <c r="D4" s="23" t="s">
         <v>156</v>
       </c>
+      <c r="E4" s="32">
+        <v>75</v>
+      </c>
+      <c r="F4" s="32">
+        <v>60</v>
+      </c>
     </row>
     <row r="5" spans="1:9" s="29" customFormat="1" ht="16" x14ac:dyDescent="0.15">
       <c r="A5" s="29" t="s">
@@ -3744,6 +3762,12 @@
       <c r="D5" s="23" t="s">
         <v>156</v>
       </c>
+      <c r="E5" s="13">
+        <v>75</v>
+      </c>
+      <c r="F5" s="13">
+        <v>60</v>
+      </c>
     </row>
     <row r="6" spans="1:9" s="29" customFormat="1" ht="16" x14ac:dyDescent="0.15">
       <c r="A6" s="29" t="s">
@@ -3758,6 +3782,12 @@
       <c r="D6" s="23" t="s">
         <v>156</v>
       </c>
+      <c r="E6" s="13">
+        <v>75</v>
+      </c>
+      <c r="F6" s="13">
+        <v>60</v>
+      </c>
     </row>
     <row r="7" spans="1:9" s="29" customFormat="1" ht="16" x14ac:dyDescent="0.15">
       <c r="A7" s="29" t="s">
@@ -3772,6 +3802,12 @@
       <c r="D7" s="23" t="s">
         <v>156</v>
       </c>
+      <c r="E7" s="13">
+        <v>75</v>
+      </c>
+      <c r="F7" s="13">
+        <v>60</v>
+      </c>
     </row>
     <row r="8" spans="1:9" s="29" customFormat="1" ht="16" x14ac:dyDescent="0.15">
       <c r="A8" s="29" t="s">
@@ -3786,6 +3822,12 @@
       <c r="D8" s="23" t="s">
         <v>156</v>
       </c>
+      <c r="E8" s="13">
+        <v>75</v>
+      </c>
+      <c r="F8" s="13">
+        <v>60</v>
+      </c>
     </row>
     <row r="9" spans="1:9" s="29" customFormat="1" ht="16" x14ac:dyDescent="0.15">
       <c r="A9" s="29" t="s">
@@ -3799,6 +3841,12 @@
       </c>
       <c r="D9" s="23" t="s">
         <v>156</v>
+      </c>
+      <c r="E9" s="13">
+        <v>75</v>
+      </c>
+      <c r="F9" s="13">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>